<commit_message>
Added & Routed RAM. Made changes to documentation file structure. Added more datasheets
</commit_message>
<xml_diff>
--- a/Hardware/Processor_Periph/Processor_BOM.xlsx
+++ b/Hardware/Processor_Periph/Processor_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Products\Laser_Cutter\Hardware\Processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Products\Laser_Cutter\Hardware\Processor_Periph\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -147,9 +147,6 @@
     <t xml:space="preserve">Q1 Q2 Q3 Q4 </t>
   </si>
   <si>
-    <t>BSSB06NE</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1 </t>
   </si>
   <si>
@@ -532,6 +529,9 @@
   </si>
   <si>
     <t xml:space="preserve">C1 C12 C14 C15 C16 C18 C21 C23 C24 C26 C27 C3 C30 C32 C33 C36 C37 C38 C39 C5 C6 C8 C9 </t>
+  </si>
+  <si>
+    <t>BSS806NE</t>
   </si>
 </sst>
 </file>
@@ -1441,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1473,13 +1473,13 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>68</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1494,16 +1494,16 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
         <v>162</v>
       </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>163</v>
-      </c>
-      <c r="H3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1518,21 +1518,21 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="4">
         <v>23</v>
@@ -1545,16 +1545,16 @@
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -1572,13 +1572,13 @@
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -1597,13 +1597,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -1622,13 +1622,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -1647,13 +1647,13 @@
         <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1672,13 +1672,13 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -1697,16 +1697,16 @@
         <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1724,16 +1724,16 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" t="s">
         <v>82</v>
       </c>
-      <c r="H12" t="s">
-        <v>83</v>
-      </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1751,16 +1751,16 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -1778,13 +1778,13 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" t="s">
         <v>118</v>
-      </c>
-      <c r="G14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1802,16 +1802,16 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" t="s">
         <v>144</v>
       </c>
-      <c r="H15" t="s">
-        <v>145</v>
-      </c>
       <c r="I15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1829,16 +1829,16 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" t="s">
         <v>76</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>77</v>
-      </c>
-      <c r="I16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1856,16 +1856,16 @@
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1883,16 +1883,16 @@
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" t="s">
         <v>76</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>77</v>
-      </c>
-      <c r="I18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1910,16 +1910,16 @@
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" t="s">
         <v>76</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>77</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1937,16 +1937,16 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1964,13 +1964,13 @@
         <v>38</v>
       </c>
       <c r="F21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" t="s">
         <v>126</v>
-      </c>
-      <c r="G21" t="s">
-        <v>125</v>
-      </c>
-      <c r="H21" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G22" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" t="s">
         <v>142</v>
-      </c>
-      <c r="H22" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -2009,24 +2009,24 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" t="s">
         <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -2036,21 +2036,21 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" t="s">
         <v>97</v>
-      </c>
-      <c r="H24" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="4">
         <v>5</v>
@@ -2060,24 +2060,24 @@
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="4">
         <v>3</v>
@@ -2087,21 +2087,21 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -2111,21 +2111,21 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4">
         <v>12</v>
@@ -2135,21 +2135,21 @@
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" t="s">
         <v>95</v>
-      </c>
-      <c r="H28" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4">
         <v>2</v>
@@ -2159,21 +2159,21 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
         <v>101</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>102</v>
-      </c>
-      <c r="H29" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
@@ -2183,21 +2183,21 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" t="s">
         <v>101</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>102</v>
-      </c>
-      <c r="H30" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
@@ -2207,21 +2207,21 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" t="s">
         <v>104</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>105</v>
-      </c>
-      <c r="H31" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
@@ -2231,21 +2231,21 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" t="s">
         <v>107</v>
-      </c>
-      <c r="G32" t="s">
-        <v>109</v>
-      </c>
-      <c r="H32" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -2255,24 +2255,24 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" t="s">
         <v>74</v>
-      </c>
-      <c r="G33" t="s">
-        <v>114</v>
-      </c>
-      <c r="H33" t="s">
-        <v>113</v>
-      </c>
-      <c r="I33" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
@@ -2282,24 +2282,24 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" t="s">
         <v>110</v>
       </c>
-      <c r="G34" t="s">
-        <v>112</v>
-      </c>
-      <c r="H34" t="s">
-        <v>111</v>
-      </c>
       <c r="I34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
@@ -2309,21 +2309,21 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" t="s">
         <v>93</v>
-      </c>
-      <c r="G35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H35" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
@@ -2333,24 +2333,24 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G36" t="s">
+        <v>157</v>
+      </c>
+      <c r="H36" t="s">
+        <v>156</v>
+      </c>
+      <c r="I36" t="s">
         <v>158</v>
-      </c>
-      <c r="H36" t="s">
-        <v>157</v>
-      </c>
-      <c r="I36" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
@@ -2360,19 +2360,19 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" t="s">
         <v>152</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>153</v>
       </c>
-      <c r="H37" t="s">
-        <v>154</v>
-      </c>
       <c r="I37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -2385,35 +2385,35 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>